<commit_message>
"Yardımcı Ekipmanlar" grubundaki Paralel Sesli Anons Model-2 olarak düzeltildi.
</commit_message>
<xml_diff>
--- a/pages/yardimci-ekipman.xlsx
+++ b/pages/yardimci-ekipman.xlsx
@@ -80,9 +80,6 @@
     <t>Kabin - Kapı Üstü</t>
   </si>
   <si>
-    <t>EQ-VOA-00-000-CLI-P1B0-01</t>
-  </si>
-  <si>
     <t>Paralel</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>Durak+8</t>
+  </si>
+  <si>
+    <t>EQ-VOA-00-000-CLI-P1B0-02</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -610,7 +610,7 @@
         <v>15</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K2" s="6"/>
     </row>
@@ -619,7 +619,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>11</v>
@@ -634,16 +634,16 @@
         <v>17</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K3" s="6"/>
     </row>
@@ -652,31 +652,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K4" s="6"/>
     </row>
@@ -685,11 +685,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
@@ -697,19 +697,19 @@
         <v>12</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K5" s="6"/>
     </row>
@@ -718,19 +718,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>13</v>
@@ -742,7 +742,7 @@
         <v>15</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6" s="6"/>
     </row>
@@ -751,31 +751,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K7" s="6"/>
     </row>
@@ -784,31 +784,31 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="J8" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K8" s="6"/>
     </row>
@@ -817,31 +817,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K9" s="6"/>
     </row>

</xml_diff>

<commit_message>
Seri ve paralel sesli anons linkleri yardımcı eleman dosyasına eklendi.
</commit_message>
<xml_diff>
--- a/pages/yardimci-ekipman.xlsx
+++ b/pages/yardimci-ekipman.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
   <si>
     <t>Sıra</t>
   </si>
@@ -153,13 +153,19 @@
   </si>
   <si>
     <t>EQ-VOA-00-000-CLI-P1B0-02</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/EQ-VOA-00-000-CLI-S2B0-02</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/EQ-VOA-00-000-CLI-P1B0-02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -198,6 +204,14 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -231,10 +245,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -244,8 +259,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,7 +544,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -542,7 +559,7 @@
     <col min="8" max="8" width="15.21875" style="1" customWidth="1"/>
     <col min="9" max="9" width="11.109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.77734375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="47.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
@@ -612,7 +629,9 @@
       <c r="J2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="6"/>
+      <c r="K2" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
@@ -645,7 +664,9 @@
       <c r="J3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="6"/>
+      <c r="K3" s="7" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
@@ -846,8 +867,12 @@
       <c r="K9" s="6"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Paralel to Seri Revizon Board için URL uzantısı eklendi.
</commit_message>
<xml_diff>
--- a/pages/yardimci-ekipman.xlsx
+++ b/pages/yardimci-ekipman.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EARGE8PC\Desktop\btk42GithubIo\pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7E5426-A53E-4925-815E-1EEE8BF42F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="46">
   <si>
     <t>Sıra</t>
   </si>
@@ -159,12 +160,15 @@
   </si>
   <si>
     <t>https://github.com/btk42/EQ-VOA-00-000-CLI-P1B0-02</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/EQ-RVB-00-PTS-REV-S3B0-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -253,8 +257,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -540,11 +544,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -559,7 +563,7 @@
     <col min="8" max="8" width="15.21875" style="1" customWidth="1"/>
     <col min="9" max="9" width="11.109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.77734375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
@@ -798,7 +802,9 @@
       <c r="J7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="6"/>
+      <c r="K7" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
@@ -868,11 +874,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="K3" r:id="rId2"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="K7" r:id="rId3" xr:uid="{49DD4C10-5C1F-4EE0-B80A-AD4887F5F67D}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>